<commit_message>
added search combos to CapStatement
</commit_message>
<xml_diff>
--- a/CapStatement/AdaptService.xlsx
+++ b/CapStatement/AdaptService.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\CapStatement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F817DED-BCE5-4BC5-84E9-AA0BE7A66238}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB77484B-0911-4180-954A-7CF50FDA6C7B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="23325" windowHeight="13980" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="-26160" yWindow="1110" windowWidth="25680" windowHeight="13875" activeTab="7" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>Value</t>
   </si>
@@ -260,6 +260,13 @@
   </si>
   <si>
     <t>http://fhir.org/guides/argonaut-questionnaire/OperationDefinition/next-question</t>
+  </si>
+  <si>
+    <t>-  The Service *SHALL* be capable of supporting  the[ Argonaut Questionnaire Profile](http://fhir.org/guides/argonaut-questionnaire/StructureDefinition/argo-questionnaire) as a contained resource with the Argonaut Adaptive QuestionnaireResponse Profile.
+-  The Service *SHALL* be capable of supporting  the[ Argonaut Questionnaire ValueSet Profile](http://fhir.org/guides/argonaut-questionnaire/StructureDefinition/argo-questionnaire-valueset) as a contained resource with the Argonaut Questionnaire Profile.</t>
+  </si>
+  <si>
+    <t>combo_pairs</t>
   </si>
 </sst>
 </file>
@@ -653,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15F3286-55C1-40D0-93FC-C97EF26956B8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACB4CFA-AAEF-4FC6-A49B-107CEE80A317}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,12 +983,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1121,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399C2ED-EDEB-47AB-8C1E-1290512B1D2F}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1145,7 @@
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1183,6 +1193,9 @@
       </c>
       <c r="P1" t="s">
         <v>34</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update jinja2 for more robust combos
</commit_message>
<xml_diff>
--- a/CapStatement/AdaptService.xlsx
+++ b/CapStatement/AdaptService.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\CapStatement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB77484B-0911-4180-954A-7CF50FDA6C7B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0752D221-1B41-4A38-A7EA-B83019D0F51E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26160" yWindow="1110" windowWidth="25680" windowHeight="13875" activeTab="7" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="-25185" yWindow="7245" windowWidth="25680" windowHeight="10665" activeTab="5" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -777,7 +777,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96A54FC-3AD5-423D-A8CA-14A00751FE64}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399C2ED-EDEB-47AB-8C1E-1290512B1D2F}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>

</xml_diff>